<commit_message>
Update lô mới về lô 26.1
</commit_message>
<xml_diff>
--- a/TDStore/OnyxtechImport.xlsx
+++ b/TDStore/OnyxtechImport.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\TDStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184C86D3-C569-4A27-AFD7-9DF07E67A305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B149DFC6-732E-4547-8017-AB14A9856DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8.1.24" sheetId="1" r:id="rId1"/>
     <sheet name="11.1.24" sheetId="2" r:id="rId2"/>
     <sheet name="24.1.24" sheetId="5" r:id="rId3"/>
     <sheet name="26.1.24" sheetId="3" r:id="rId4"/>
-    <sheet name="07.02.24" sheetId="7" r:id="rId5"/>
+    <sheet name="1.2.24" sheetId="8" r:id="rId5"/>
+    <sheet name="07.02.24" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
   <si>
     <t>Tên máy</t>
   </si>
@@ -138,6 +139,24 @@
   <si>
     <t>1Z 538 V5V 03 5380 3444
 1Z 538 V5V 03 2047 0811</t>
+  </si>
+  <si>
+    <t>7420</t>
+  </si>
+  <si>
+    <t>7410 Bad</t>
+  </si>
+  <si>
+    <t>A2152</t>
+  </si>
+  <si>
+    <t>Thiếu</t>
+  </si>
+  <si>
+    <t>9405511206217728792385 9405511206217728794570 9405511206217728794358 9405511206217728793108</t>
+  </si>
+  <si>
+    <t>Cam</t>
   </si>
 </sst>
 </file>
@@ -153,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +194,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -228,6 +253,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -521,11 +565,12 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="5" max="5" width="16.3984375" customWidth="1"/>
     <col min="6" max="6" width="24.3984375" customWidth="1"/>
-    <col min="7" max="7" width="33.59765625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.3984375" customWidth="1"/>
+    <col min="7" max="7" width="24.3984375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="33.59765625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="22.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -544,43 +589,49 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="15">
         <v>7390</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="16">
         <v>70</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="16">
         <f>25000*B2</f>
         <v>1750000</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="16">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="16">
         <f>B2*D2</f>
         <v>210</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="19">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>2188000</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>7400</v>
       </c>
@@ -599,34 +650,40 @@
         <v>85</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="18">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="15">
         <v>7420</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="16">
         <v>120</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="16">
         <f t="shared" si="0"/>
         <v>3000000</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>7740</v>
       </c>
@@ -645,8 +702,9 @@
         <v>300</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>7410</v>
       </c>
@@ -665,16 +723,18 @@
         <v>100</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -687,11 +747,11 @@
         <f>SUM(E2:E6)</f>
         <v>815</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -701,7 +761,7 @@
         <f>SUM(C2:C6)</f>
         <v>16875000</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -715,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -903,7 +963,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1090,10 +1150,276 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.86328125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="5" max="6" width="16.3984375" customWidth="1"/>
+    <col min="7" max="8" width="15.1328125" customWidth="1"/>
+    <col min="9" max="9" width="28.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8">
+        <v>110</v>
+      </c>
+      <c r="C2" s="8">
+        <f>25000*B2</f>
+        <v>2750000</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <f>B2*D2</f>
+        <v>220</v>
+      </c>
+      <c r="F2" s="8">
+        <v>3</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="23">
+        <v>85</v>
+      </c>
+      <c r="C3" s="23">
+        <f t="shared" ref="C3:C8" si="0">25000*B3</f>
+        <v>2125000</v>
+      </c>
+      <c r="D3" s="23">
+        <v>5</v>
+      </c>
+      <c r="E3" s="23">
+        <f t="shared" ref="E3:E8" si="1">B3*D3</f>
+        <v>425</v>
+      </c>
+      <c r="F3" s="23">
+        <v>3</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8">
+        <v>450</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="0"/>
+        <v>11250000</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="8">
+        <v>300</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
+        <v>7500000</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="23">
+        <v>40</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="F6" s="23">
+        <v>0</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="22">
+        <v>7420</v>
+      </c>
+      <c r="B7" s="23">
+        <v>120</v>
+      </c>
+      <c r="C7" s="23">
+        <f t="shared" si="0"/>
+        <v>3000000</v>
+      </c>
+      <c r="D7" s="23">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="F7" s="23">
+        <v>0</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8">
+        <v>65</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" si="0"/>
+        <v>1625000</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="10">
+        <f>SUM(E2:E8)</f>
+        <v>1685</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="10">
+        <f>SUM(C2:C6)</f>
+        <v>24625000</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52BB421-245D-4FCF-8A03-DD59F425FDF8}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1102,11 +1428,11 @@
     <col min="2" max="2" width="12.86328125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="5" max="5" width="16.3984375" customWidth="1"/>
-    <col min="6" max="7" width="15.1328125" customWidth="1"/>
-    <col min="8" max="8" width="28.73046875" customWidth="1"/>
+    <col min="6" max="6" width="15.1328125" customWidth="1"/>
+    <col min="9" max="9" width="28.73046875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1125,39 +1451,39 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="6"/>
+      <c r="I1" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C2" s="8">
         <f>25000*B2</f>
-        <v>2750000</v>
+        <v>1875000</v>
       </c>
       <c r="D2" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="8">
         <f>B2*D2</f>
-        <v>220</v>
+        <v>75</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G2" s="6"/>
+      <c r="I2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -1165,168 +1491,239 @@
         <v>85</v>
       </c>
       <c r="C3" s="8">
-        <f t="shared" ref="C3:C8" si="0">25000*B3</f>
+        <f t="shared" ref="C3" si="0">25000*B3</f>
         <v>2125000</v>
       </c>
       <c r="D3" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" ref="E3:E8" si="1">B3*D3</f>
-        <v>425</v>
+        <f t="shared" ref="E3" si="1">B3*D3</f>
+        <v>85</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G3" s="6"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="8">
-        <v>450</v>
+        <v>110</v>
       </c>
       <c r="C4" s="8">
-        <f t="shared" si="0"/>
-        <v>11250000</v>
+        <f t="shared" ref="C4:C11" si="2">25000*B4</f>
+        <v>2750000</v>
       </c>
       <c r="D4" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" si="1"/>
-        <v>450</v>
+        <f t="shared" ref="E4:E11" si="3">B4*D4</f>
+        <v>330</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8">
+        <v>50</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="2"/>
+        <v>1250000</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8">
+        <v>120</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="2"/>
+        <v>3000000</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="7">
+        <v>7390</v>
+      </c>
+      <c r="B7" s="8">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="2"/>
+        <v>1250000</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="7">
+        <v>7280</v>
+      </c>
+      <c r="B8" s="8">
+        <v>55</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" si="2"/>
+        <v>1375000</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="8">
+        <v>250</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="2"/>
+        <v>6250000</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8">
+        <v>290</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="2"/>
+        <v>7250000</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="3"/>
+        <v>870</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="8">
         <v>300</v>
       </c>
-      <c r="C5" s="8">
-        <f t="shared" si="0"/>
+      <c r="C11" s="8">
+        <f t="shared" si="2"/>
         <v>7500000</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8">
-        <f t="shared" si="1"/>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="8">
-        <v>40</v>
-      </c>
-      <c r="C6" s="8">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="7">
-        <v>7420</v>
-      </c>
-      <c r="B7" s="8">
-        <v>120</v>
-      </c>
-      <c r="C7" s="8">
-        <f t="shared" si="0"/>
-        <v>3000000</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="8">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="8">
-        <v>65</v>
-      </c>
-      <c r="C8" s="8">
-        <f t="shared" si="0"/>
-        <v>1625000</v>
-      </c>
-      <c r="D8" s="8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="8">
-        <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="10">
-        <f>SUM(E2:E8)</f>
-        <v>1685</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8">
+        <f>SUM(D2:D11)</f>
+        <v>15</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8">
+        <f>SUM(E2:E11)</f>
+        <v>2235</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="10">
-        <f>SUM(C2:C6)</f>
-        <v>24625000</v>
-      </c>
-      <c r="F11" s="11" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8">
+        <f>SUM(C2:C7)</f>
+        <v>12250000</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B97A4A5-F0C2-4EC0-B0E6-B64B83A23504}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>